<commit_message>
poeple import and people重点人员识别记录
</commit_message>
<xml_diff>
--- a/Service/People/src/main/resources/excel/people_excel.xlsx
+++ b/Service/People/src/main/resources/excel/people_excel.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zz\zz20181106\GoSunBigData\Service\People\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zz\zz20181119\GoSunBigData\Service\People\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9598EC0E-C2AE-4190-B0D6-2F3862A247A8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B795E-D1D2-434D-8356-657CCB1F81D6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="侦码后台信息" sheetId="3" r:id="rId1"/>
+    <sheet name="人口库导入" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -509,7 +509,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>